<commit_message>
finished q1 & q2
</commit_message>
<xml_diff>
--- a/Assignments/hw1/q1fp/q1fp.xlsx
+++ b/Assignments/hw1/q1fp/q1fp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Aero_5830\Assignments\hw1\q1fp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AD3ABFE-401B-4F21-8C77-DA92F696A969}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F31EEF-BCCC-4C3A-A987-DE4E0C4655FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{1A648A2D-4EB8-45EF-AC20-A492F9B10A5D}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$B$1:$B$9</definedName>
-    <definedName name="ExternalData_2" localSheetId="0" hidden="1">Sheet1!$C$1:$C$9</definedName>
-    <definedName name="ExternalData_3" localSheetId="0" hidden="1">Sheet1!$D$1:$D$8</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$B$1:$B$10</definedName>
+    <definedName name="ExternalData_2" localSheetId="0" hidden="1">Sheet1!$D$1:$D$10</definedName>
+    <definedName name="ExternalData_3" localSheetId="0" hidden="1">Sheet1!$E$1:$E$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,75 +53,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>3.4063696853821592</t>
-  </si>
-  <si>
-    <t>3.5654912012141353</t>
-  </si>
-  <si>
-    <t>3.5393882796306126</t>
-  </si>
-  <si>
-    <t>3.544837003122535</t>
-  </si>
-  <si>
-    <t>3.5449068645481048</t>
-  </si>
-  <si>
-    <t>3.5449076919059457</t>
-  </si>
-  <si>
-    <t>3.544907701693853</t>
-  </si>
-  <si>
-    <t>-8.704481115988136</t>
-  </si>
-  <si>
-    <t>1.708125012744465</t>
-  </si>
-  <si>
-    <t>-0.4506154556475088</t>
-  </si>
-  <si>
-    <t>-0.0057972258410804835</t>
-  </si>
-  <si>
-    <t>-6.865839064142679e-05</t>
-  </si>
-  <si>
-    <t>-8.122510793581068e-07</t>
-  </si>
-  <si>
-    <t>-9.60908294510742e-09</t>
-  </si>
-  <si>
-    <t>0.1874999999999999</t>
-  </si>
-  <si>
-    <t>0.10358692489943173</t>
-  </si>
-  <si>
-    <t>0.0467129321032941</t>
-  </si>
-  <si>
-    <t>0.007320988921423787</t>
-  </si>
-  <si>
-    <t>0.0015394534482921789</t>
-  </si>
-  <si>
-    <t>1.9707937348973396e-05</t>
-  </si>
-  <si>
-    <t>2.3339339297707222e-07</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>iteration (n)</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>t_n</t>
@@ -137,6 +71,9 @@
   </si>
   <si>
     <t>3.2-3.8</t>
+  </si>
+  <si>
+    <t>t_n+1</t>
   </si>
 </sst>
 </file>
@@ -184,16 +121,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -218,9 +159,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{F336CA1A-8B08-411F-85A7-84BB148D234C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="2">
-    <queryTableFields count="1">
+  <queryTableRefresh nextId="3" unboundColumnsRight="1">
+    <queryTableFields count="2">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
+      <queryTableField id="2" dataBound="0" tableColumnId="2"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -247,28 +189,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2752E38-93DD-4AA6-85B0-AFA5BCCE078C}" name="cl" displayName="cl" ref="B1:B9" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="B1:B9" xr:uid="{B1D00F2F-F55C-4F25-9DB6-0450BE238D1D}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2752E38-93DD-4AA6-85B0-AFA5BCCE078C}" name="cl" displayName="cl" ref="B1:C10" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="B1:C10" xr:uid="{B1D00F2F-F55C-4F25-9DB6-0450BE238D1D}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E7EAC9B8-C2B7-4418-91AB-69ED5A71182C}" uniqueName="1" name="t_n" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5BB137D7-CEA4-4549-990A-DF6AA52167CB}" uniqueName="2" name="t_n+1" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{66D75D54-F9FF-494D-9740-FE390B50B141}" name="fl" displayName="fl" ref="C1:C9" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="C1:C9" xr:uid="{B851C7A7-BFF8-4F85-9C7A-CEAF9A006604}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{66D75D54-F9FF-494D-9740-FE390B50B141}" name="fl" displayName="fl" ref="D1:D10" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="D1:D10" xr:uid="{B851C7A7-BFF8-4F85-9C7A-CEAF9A006604}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A130192D-6907-47EC-B057-DA9F7A4D72CA}" uniqueName="1" name="f(n)" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A130192D-6907-47EC-B057-DA9F7A4D72CA}" uniqueName="1" name="f(n)" queryTableFieldId="1" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{345D8DC3-A397-436B-AFAA-DA0AAEAC6A5B}" name="eps" displayName="eps" ref="D1:D8" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="D1:D8" xr:uid="{6CA9D4C6-E09E-414B-A235-E2850F8BC4A0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{345D8DC3-A397-436B-AFAA-DA0AAEAC6A5B}" name="eps" displayName="eps" ref="E1:E9" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="E1:E9" xr:uid="{6CA9D4C6-E09E-414B-A235-E2850F8BC4A0}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{58F43370-888E-4D86-BFD5-D2DCE02BAF73}" uniqueName="1" name="eps_n" queryTableFieldId="1" dataDxfId="2"/>
   </tableColumns>
@@ -573,149 +516,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D3C60-313D-4A88-9D7B-DD806B3CF5E7}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F18"/>
+      <selection activeCell="D16" sqref="B15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>3.2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="D2">
+        <v>-6.7255915220315696</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.187499999999999</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.4063696853821499</v>
+      </c>
+      <c r="D3" s="1">
+        <v>12.8284185824379</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.103586924899431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>3.4063696853821499</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.56549120121413</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-8.7044811159881306</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4.6712932103294101E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3.56549120121413</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.53938827963061</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.70812501274446</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7.3209889214237798E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>3.53938827963061</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.54483700312253</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-0.45061545564750799</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.53945344829217E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3.54483700312253</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.5449068645480999</v>
+      </c>
+      <c r="D7" s="4">
+        <v>-5.79722584108048E-3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.9707937348973301E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>3.5449068645480999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.5449076919059399</v>
+      </c>
+      <c r="D8" s="4">
+        <v>-6.8658390641426696E-5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2.3339339297707201E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B9" s="1">
+        <v>3.5449076919059399</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.5449077016938499</v>
+      </c>
+      <c r="D9" s="4">
+        <v>-8.1225107935810598E-7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2.7611177001425499E-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>3.5449077016938499</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <v>-9.6090829451074196E-9</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>